<commit_message>
added complete training pipeline-1
</commit_message>
<xml_diff>
--- a/artifacts/data_ingestion/Lstm_Dates.xlsx
+++ b/artifacts/data_ingestion/Lstm_Dates.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1994"/>
+  <dimension ref="A1:C2000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22813,7 +22813,7 @@
       </c>
       <c r="B1991" t="inlineStr"/>
       <c r="C1991" t="n">
-        <v>219.0825</v>
+        <v>216.89</v>
       </c>
     </row>
     <row r="1992">
@@ -22822,16 +22822,20 @@
       </c>
       <c r="B1992" t="inlineStr"/>
       <c r="C1992" t="n">
-        <v>219.165</v>
+        <v>214.78</v>
       </c>
     </row>
     <row r="1993">
       <c r="A1993" s="2" t="n">
         <v>45607</v>
       </c>
-      <c r="B1993" t="inlineStr"/>
+      <c r="B1993" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
       <c r="C1993" t="n">
-        <v>219.2475</v>
+        <v>212.67</v>
       </c>
     </row>
     <row r="1994">
@@ -22845,6 +22849,72 @@
       </c>
       <c r="C1994" t="n">
         <v>219.33</v>
+      </c>
+    </row>
+    <row r="1995">
+      <c r="A1995" s="2" t="n">
+        <v>45609</v>
+      </c>
+      <c r="B1995" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C1995" t="n">
+        <v>219.33</v>
+      </c>
+    </row>
+    <row r="1996">
+      <c r="A1996" s="2" t="n">
+        <v>45610</v>
+      </c>
+      <c r="B1996" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C1996" t="n">
+        <v>217.67</v>
+      </c>
+    </row>
+    <row r="1997">
+      <c r="A1997" s="2" t="n">
+        <v>45611</v>
+      </c>
+      <c r="B1997" t="inlineStr"/>
+      <c r="C1997" t="n">
+        <v>218.67</v>
+      </c>
+    </row>
+    <row r="1998">
+      <c r="A1998" s="2" t="n">
+        <v>45612</v>
+      </c>
+      <c r="B1998" t="inlineStr"/>
+      <c r="C1998" t="n">
+        <v>219.67</v>
+      </c>
+    </row>
+    <row r="1999">
+      <c r="A1999" s="2" t="n">
+        <v>45613</v>
+      </c>
+      <c r="B1999" t="inlineStr"/>
+      <c r="C1999" t="n">
+        <v>220.67</v>
+      </c>
+    </row>
+    <row r="2000">
+      <c r="A2000" s="2" t="n">
+        <v>45614</v>
+      </c>
+      <c r="B2000" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C2000" t="n">
+        <v>221.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new training pipeline
</commit_message>
<xml_diff>
--- a/artifacts/data_ingestion/Lstm_Dates.xlsx
+++ b/artifacts/data_ingestion/Lstm_Dates.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2000"/>
+  <dimension ref="A1:C2001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22917,6 +22917,19 @@
         <v>221.67</v>
       </c>
     </row>
+    <row r="2001">
+      <c r="A2001" s="2" t="n">
+        <v>45615</v>
+      </c>
+      <c r="B2001" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C2001" t="n">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added the 3 pipelines
</commit_message>
<xml_diff>
--- a/artifacts/data_ingestion/Lstm_Dates.xlsx
+++ b/artifacts/data_ingestion/Lstm_Dates.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2001"/>
+  <dimension ref="A1:C2002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22930,6 +22930,19 @@
         <v>226</v>
       </c>
     </row>
+    <row r="2002">
+      <c r="A2002" s="2" t="n">
+        <v>45616</v>
+      </c>
+      <c r="B2002" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C2002" t="n">
+        <v>225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added the dockerfile and streamlit UI
</commit_message>
<xml_diff>
--- a/artifacts/data_ingestion/Lstm_Dates.xlsx
+++ b/artifacts/data_ingestion/Lstm_Dates.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2002"/>
+  <dimension ref="A1:C2004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5025,7 +5025,7 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>92.59999999999999</v>
+        <v>92.8</v>
       </c>
     </row>
     <row r="416">
@@ -5034,7 +5034,7 @@
       </c>
       <c r="B416" t="inlineStr"/>
       <c r="C416" t="n">
-        <v>92.65000000000001</v>
+        <v>92.8</v>
       </c>
     </row>
     <row r="417">
@@ -5043,7 +5043,7 @@
       </c>
       <c r="B417" t="inlineStr"/>
       <c r="C417" t="n">
-        <v>92.7</v>
+        <v>92.8</v>
       </c>
     </row>
     <row r="418">
@@ -5052,7 +5052,7 @@
       </c>
       <c r="B418" t="inlineStr"/>
       <c r="C418" t="n">
-        <v>92.75</v>
+        <v>92.8</v>
       </c>
     </row>
     <row r="419">
@@ -22941,6 +22941,32 @@
       </c>
       <c r="C2002" t="n">
         <v>225</v>
+      </c>
+    </row>
+    <row r="2003">
+      <c r="A2003" s="2" t="n">
+        <v>45617</v>
+      </c>
+      <c r="B2003" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C2003" t="n">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2004">
+      <c r="A2004" s="2" t="n">
+        <v>45618</v>
+      </c>
+      <c r="B2004" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C2004" t="n">
+        <v>220.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleane the code to make up to production level
</commit_message>
<xml_diff>
--- a/artifacts/data_ingestion/Lstm_Dates.xlsx
+++ b/artifacts/data_ingestion/Lstm_Dates.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2004"/>
+  <dimension ref="A1:C2014"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22969,6 +22969,120 @@
         <v>220.67</v>
       </c>
     </row>
+    <row r="2005">
+      <c r="A2005" s="2" t="n">
+        <v>45619</v>
+      </c>
+      <c r="B2005" t="inlineStr"/>
+      <c r="C2005" t="n">
+        <v>223.5566666666667</v>
+      </c>
+    </row>
+    <row r="2006">
+      <c r="A2006" s="2" t="n">
+        <v>45620</v>
+      </c>
+      <c r="B2006" t="inlineStr"/>
+      <c r="C2006" t="n">
+        <v>226.4433333333333</v>
+      </c>
+    </row>
+    <row r="2007">
+      <c r="A2007" s="2" t="n">
+        <v>45621</v>
+      </c>
+      <c r="B2007" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C2007" t="n">
+        <v>229.33</v>
+      </c>
+    </row>
+    <row r="2008">
+      <c r="A2008" s="2" t="n">
+        <v>45622</v>
+      </c>
+      <c r="B2008" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C2008" t="n">
+        <v>229.33</v>
+      </c>
+    </row>
+    <row r="2009">
+      <c r="A2009" s="2" t="n">
+        <v>45623</v>
+      </c>
+      <c r="B2009" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C2009" t="n">
+        <v>228.33</v>
+      </c>
+    </row>
+    <row r="2010">
+      <c r="A2010" s="2" t="n">
+        <v>45624</v>
+      </c>
+      <c r="B2010" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C2010" t="n">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2011">
+      <c r="A2011" s="2" t="n">
+        <v>45625</v>
+      </c>
+      <c r="B2011" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C2011" t="n">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2012">
+      <c r="A2012" s="2" t="n">
+        <v>45626</v>
+      </c>
+      <c r="B2012" t="inlineStr"/>
+      <c r="C2012" t="n">
+        <v>231.5</v>
+      </c>
+    </row>
+    <row r="2013">
+      <c r="A2013" s="2" t="n">
+        <v>45627</v>
+      </c>
+      <c r="B2013" t="inlineStr"/>
+      <c r="C2013" t="n">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2014">
+      <c r="A2014" s="2" t="n">
+        <v>45628</v>
+      </c>
+      <c r="B2014" t="inlineStr">
+        <is>
+          <t>Nadu 2</t>
+        </is>
+      </c>
+      <c r="C2014" t="n">
+        <v>236.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>